<commit_message>
Frequent Flyer shit works
</commit_message>
<xml_diff>
--- a/FFlyer/Formulas.xlsx
+++ b/FFlyer/Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kpmgaust-my.sharepoint.com/personal/jhansen3_kpmg_com_au/Documents/Documents/Python/Gambling/FFlyer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_7F8F7014B01395E076ECEF001A449A64D5F6B63D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F185257-DA87-43EE-88BF-420EF0844785}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_7F8F7014B01395E076ECEF001A449A64D5F6B63D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E49BA4A0-4D6F-4A16-940E-8D6EF8B894F6}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$B$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$B$2:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Test!$B$2:$H$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -480,679 +480,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I573"/>
+  <dimension ref="B2:J573"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="66.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="19.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="8" customWidth="1"/>
+    <col min="5" max="10" width="19.88671875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
+        <f>DATE(RIGHT(C3, 4), LEFT(C3, 2), MID(C3, 4, 2))</f>
+        <v>45319</v>
+      </c>
+      <c r="E3" s="2">
         <v>92200</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>584</v>
       </c>
-      <c r="G3" s="8" t="str">
-        <f>IF(D3&gt;(2*_xlfn.XLOOKUP(B3, B:B, D:D)), "Yes", "No")</f>
+      <c r="H3" s="8" t="str">
+        <f>IF(E3&gt;(2*_xlfn.XLOOKUP(B3, B:B, E:E)), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="H3" s="8">
-        <f>(F3-E3)/(D3/1000)</f>
+      <c r="I3" s="8">
+        <f>(G3-F3)/(E3/1000)</f>
         <v>4.7232104121475054</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D24" si="0">DATE(RIGHT(C4, 4), LEFT(C4, 2), MID(C4, 4, 2))</f>
+        <v>45319</v>
+      </c>
+      <c r="E4" s="2">
         <v>117100</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>584</v>
       </c>
-      <c r="G4" s="8" t="str">
-        <f t="shared" ref="G4:G24" si="0">IF(D4&gt;(2*_xlfn.XLOOKUP(B4, B:B, D:D)), "Yes", "No")</f>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ref="H4:H24" si="1">IF(E4&gt;(2*_xlfn.XLOOKUP(B4, B:B, E:E)), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="H4" s="8">
-        <f>(F4-E4)/(D4/1000)</f>
+      <c r="I4" s="8">
+        <f t="shared" ref="I4:I24" si="2">(G4-F4)/(E4/1000)</f>
         <v>4.9871904355251928</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E5" s="2">
         <v>92200</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>584</v>
       </c>
-      <c r="G5" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H5" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H5" s="8">
-        <f>(F5-E5)/(D5/1000)</f>
+      <c r="I5" s="8">
+        <f t="shared" si="2"/>
         <v>4.7232104121475054</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E6" s="2">
         <v>117100</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>584</v>
       </c>
-      <c r="G6" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H6" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H6" s="8">
-        <f>(F6-E6)/(D6/1000)</f>
+      <c r="I6" s="8">
+        <f t="shared" si="2"/>
         <v>4.9871904355251928</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E7" s="2">
         <v>108400</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>584</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H7" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H7" s="8">
-        <f>(F7-E7)/(D7/1000)</f>
+      <c r="I7" s="8">
+        <f t="shared" si="2"/>
         <v>4.0173431734317342</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E8" s="2">
         <v>133300</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>584</v>
       </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H8" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H8" s="8">
-        <f>(F8-E8)/(D8/1000)</f>
+      <c r="I8" s="8">
+        <f t="shared" si="2"/>
         <v>4.3810952738184543</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E9" s="2">
         <v>253000</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>584</v>
       </c>
-      <c r="G9" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H9" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H9" s="8">
-        <f>(F9-E9)/(D9/1000)</f>
+      <c r="I9" s="8">
+        <f t="shared" si="2"/>
         <v>1.7212648221343874</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E10" s="2">
         <v>277900</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>584</v>
       </c>
-      <c r="G10" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H10" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H10" s="8">
-        <f>(F10-E10)/(D10/1000)</f>
+      <c r="I10" s="8">
+        <f t="shared" si="2"/>
         <v>2.1014753508456283</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E11" s="2">
         <v>75000</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>11</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1403</v>
       </c>
-      <c r="G11" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H11" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H11" s="8">
-        <f>(F11-E11)/(D11/1000)</f>
+      <c r="I11" s="8">
+        <f t="shared" si="2"/>
         <v>14.511466666666669</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E12" s="2">
         <v>127600</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1403</v>
       </c>
-      <c r="G12" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H12" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H12" s="8">
-        <f>(F12-E12)/(D12/1000)</f>
+      <c r="I12" s="8">
+        <f t="shared" si="2"/>
         <v>10.995297805642634</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E13" s="2">
         <v>159900</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1403</v>
       </c>
-      <c r="G13" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H13" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H13" s="8">
-        <f>(F13-E13)/(D13/1000)</f>
+      <c r="I13" s="8">
+        <f t="shared" si="2"/>
         <v>5.994121325828643</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E14" s="2">
         <v>234100</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1403</v>
       </c>
-      <c r="G14" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H14" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H14" s="8">
-        <f>(F14-E14)/(D14/1000)</f>
+      <c r="I14" s="8">
+        <f t="shared" si="2"/>
         <v>5.9931653139683894</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E15" s="2">
         <v>1143200</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1403</v>
       </c>
-      <c r="G15" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H15" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H15" s="8">
-        <f>(F15-E15)/(D15/1000)</f>
+      <c r="I15" s="8">
+        <f t="shared" si="2"/>
         <v>0.65995451364590618</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>45319</v>
+      </c>
+      <c r="E16" s="2">
         <v>1251400</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1403</v>
       </c>
-      <c r="G16" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H16" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H16" s="8">
-        <f>(F16-E16)/(D16/1000)</f>
+      <c r="I16" s="8">
+        <f t="shared" si="2"/>
         <v>1.1211443183634329</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E17" s="2">
         <v>22300</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>584</v>
       </c>
-      <c r="G17" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H17" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H17" s="8">
-        <f>(F17-E17)/(D17/1000)</f>
+      <c r="I17" s="8">
+        <f t="shared" si="2"/>
         <v>17.510313901345292</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E18" s="2">
         <v>54700</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>584</v>
       </c>
-      <c r="G18" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H18" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H18" s="8">
-        <f>(F18-E18)/(D18/1000)</f>
+      <c r="I18" s="8">
+        <f t="shared" si="2"/>
         <v>10.676416819012797</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E19" s="2">
         <v>92200</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>9</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>584</v>
       </c>
-      <c r="G19" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H19" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H19" s="8">
-        <f>(F19-E19)/(D19/1000)</f>
+      <c r="I19" s="8">
+        <f t="shared" si="2"/>
         <v>4.7232104121475054</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E20" s="2">
         <v>117100</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>584</v>
       </c>
-      <c r="G20" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H20" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H20" s="8">
-        <f>(F20-E20)/(D20/1000)</f>
+      <c r="I20" s="8">
+        <f t="shared" si="2"/>
         <v>4.9871904355251928</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E21" s="2">
         <v>92200</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>9</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>584</v>
       </c>
-      <c r="G21" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H21" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H21" s="8">
-        <f>(F21-E21)/(D21/1000)</f>
+      <c r="I21" s="8">
+        <f t="shared" si="2"/>
         <v>4.7232104121475054</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E22" s="2">
         <v>117100</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>584</v>
       </c>
-      <c r="G22" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H22" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H22" s="8">
-        <f>(F22-E22)/(D22/1000)</f>
+      <c r="I22" s="8">
+        <f t="shared" si="2"/>
         <v>4.9871904355251928</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E23" s="2">
         <v>356000</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>9</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>584</v>
       </c>
-      <c r="G23" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H23" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H23" s="8">
-        <f>(F23-E23)/(D23/1000)</f>
+      <c r="I23" s="8">
+        <f t="shared" si="2"/>
         <v>1.2232584269662923</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="E24" s="2">
         <v>380900</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>584</v>
       </c>
-      <c r="G24" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H24" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H24" s="8">
-        <f>(F24-E24)/(D24/1000)</f>
+      <c r="I24" s="8">
+        <f t="shared" si="2"/>
         <v>1.5332108164872671</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D46" s="6"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="80" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D80" s="6"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="7"/>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D81" s="2"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="9"/>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D82" s="2"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="9"/>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D84" s="2"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="9"/>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D98" s="2"/>
-      <c r="F98" s="9"/>
-    </row>
-    <row r="201" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D201" s="2"/>
-      <c r="F201" s="9"/>
-    </row>
-    <row r="204" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D204" s="2"/>
-      <c r="F204" s="9"/>
-    </row>
-    <row r="276" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D276" s="2"/>
-      <c r="E276" s="4"/>
-      <c r="F276" s="9"/>
-    </row>
-    <row r="290" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D290" s="2"/>
-      <c r="F290" s="9"/>
-    </row>
-    <row r="293" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D293" s="2"/>
-      <c r="F293" s="9"/>
-    </row>
-    <row r="299" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D299" s="2"/>
-      <c r="E299" s="4"/>
-      <c r="F299" s="9"/>
-    </row>
-    <row r="305" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D305" s="2"/>
-      <c r="F305" s="9"/>
-    </row>
-    <row r="317" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D317" s="2"/>
-      <c r="F317" s="9"/>
-    </row>
-    <row r="321" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D321" s="2"/>
-      <c r="E321" s="4"/>
-      <c r="F321" s="9"/>
-    </row>
-    <row r="391" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D391" s="2"/>
-      <c r="F391" s="9"/>
-    </row>
-    <row r="392" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D392" s="2"/>
-      <c r="F392" s="9"/>
-    </row>
-    <row r="393" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D393" s="2"/>
-      <c r="E393" s="4"/>
-      <c r="F393" s="9"/>
-    </row>
-    <row r="394" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D394" s="2"/>
-      <c r="E394" s="4"/>
-      <c r="F394" s="9"/>
-    </row>
-    <row r="447" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D447" s="2"/>
-      <c r="F447" s="9"/>
-    </row>
-    <row r="449" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D449" s="2"/>
-      <c r="F449" s="9"/>
-    </row>
-    <row r="451" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D451" s="2"/>
-      <c r="E451" s="4"/>
-      <c r="F451" s="9"/>
-    </row>
-    <row r="474" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D474" s="2"/>
-      <c r="F474" s="9"/>
-    </row>
-    <row r="573" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D573" s="2"/>
-      <c r="E573" s="4"/>
-      <c r="F573" s="9"/>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="6"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="2"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="2"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E80" s="6"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E81" s="2"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="9"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E82" s="2"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="9"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E84" s="2"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="9"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E98" s="2"/>
+      <c r="G98" s="9"/>
+    </row>
+    <row r="201" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E201" s="2"/>
+      <c r="G201" s="9"/>
+    </row>
+    <row r="204" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E204" s="2"/>
+      <c r="G204" s="9"/>
+    </row>
+    <row r="276" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E276" s="2"/>
+      <c r="F276" s="4"/>
+      <c r="G276" s="9"/>
+    </row>
+    <row r="290" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E290" s="2"/>
+      <c r="G290" s="9"/>
+    </row>
+    <row r="293" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E293" s="2"/>
+      <c r="G293" s="9"/>
+    </row>
+    <row r="299" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E299" s="2"/>
+      <c r="F299" s="4"/>
+      <c r="G299" s="9"/>
+    </row>
+    <row r="305" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E305" s="2"/>
+      <c r="G305" s="9"/>
+    </row>
+    <row r="317" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E317" s="2"/>
+      <c r="G317" s="9"/>
+    </row>
+    <row r="321" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E321" s="2"/>
+      <c r="F321" s="4"/>
+      <c r="G321" s="9"/>
+    </row>
+    <row r="391" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E391" s="2"/>
+      <c r="G391" s="9"/>
+    </row>
+    <row r="392" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E392" s="2"/>
+      <c r="G392" s="9"/>
+    </row>
+    <row r="393" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E393" s="2"/>
+      <c r="F393" s="4"/>
+      <c r="G393" s="9"/>
+    </row>
+    <row r="394" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E394" s="2"/>
+      <c r="F394" s="4"/>
+      <c r="G394" s="9"/>
+    </row>
+    <row r="447" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E447" s="2"/>
+      <c r="G447" s="9"/>
+    </row>
+    <row r="449" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E449" s="2"/>
+      <c r="G449" s="9"/>
+    </row>
+    <row r="451" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E451" s="2"/>
+      <c r="F451" s="4"/>
+      <c r="G451" s="9"/>
+    </row>
+    <row r="474" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E474" s="2"/>
+      <c r="G474" s="9"/>
+    </row>
+    <row r="573" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E573" s="2"/>
+      <c r="F573" s="4"/>
+      <c r="G573" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B2:J2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>

</xml_diff>